<commit_message>
weeks 9 and 10
</commit_message>
<xml_diff>
--- a/nfl/results/results.xlsx
+++ b/nfl/results/results.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="1120" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="2080" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId5"/>
-    <pivotCache cacheId="11" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="77">
   <si>
     <t>train</t>
   </si>
@@ -128,6 +130,135 @@
   </si>
   <si>
     <t>average</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>favorite</t>
+  </si>
+  <si>
+    <t>underdog</t>
+  </si>
+  <si>
+    <t>absLine</t>
+  </si>
+  <si>
+    <t>predict_proba</t>
+  </si>
+  <si>
+    <t>predictWin</t>
+  </si>
+  <si>
+    <t>Kansas City Chiefs</t>
+  </si>
+  <si>
+    <t>Jacksonville Jaguars</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys</t>
+  </si>
+  <si>
+    <t>Cleveland Browns</t>
+  </si>
+  <si>
+    <t>Minnesota Vikings</t>
+  </si>
+  <si>
+    <t>Detroit Lions</t>
+  </si>
+  <si>
+    <t>Green Bay Packers</t>
+  </si>
+  <si>
+    <t>Indianapolis Colts</t>
+  </si>
+  <si>
+    <t>Seattle Seahawks</t>
+  </si>
+  <si>
+    <t>Buffalo Bills</t>
+  </si>
+  <si>
+    <t>Atlanta Falcons</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers</t>
+  </si>
+  <si>
+    <t>New Orleans Saints</t>
+  </si>
+  <si>
+    <t>San Francisco 49ers</t>
+  </si>
+  <si>
+    <t>New York Giants</t>
+  </si>
+  <si>
+    <t>Philadelphia Eagles</t>
+  </si>
+  <si>
+    <t>Miami Dolphins</t>
+  </si>
+  <si>
+    <t>New York Jets</t>
+  </si>
+  <si>
+    <t>San Diego Chargers</t>
+  </si>
+  <si>
+    <t>Tennessee Titans</t>
+  </si>
+  <si>
+    <t>Carolina Panthers</t>
+  </si>
+  <si>
+    <t>Los Angeles Rams</t>
+  </si>
+  <si>
+    <t>Oakland Raiders</t>
+  </si>
+  <si>
+    <t>Denver Broncos</t>
+  </si>
+  <si>
+    <t>Baltimore Ravens</t>
+  </si>
+  <si>
+    <t>Pittsburgh Steelers</t>
+  </si>
+  <si>
+    <t>Spread</t>
+  </si>
+  <si>
+    <t>Spread rank</t>
+  </si>
+  <si>
+    <t>Favorite</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Probability of winning</t>
+  </si>
+  <si>
+    <t>Predicted team</t>
+  </si>
+  <si>
+    <t>Predicted win</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Favored win</t>
   </si>
 </sst>
 </file>
@@ -137,7 +268,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,8 +316,19 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,8 +347,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -298,8 +470,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -337,8 +524,82 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -388,8 +649,45 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -408,6 +706,43 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -426,9 +761,52 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -440,12 +818,6 @@
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
@@ -1030,7 +1402,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" printDrill="1" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" printDrill="1" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G12" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -1122,20 +1494,20 @@
     <format dxfId="6">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="5">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="4">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -1149,7 +1521,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1231,7 +1603,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G11" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -1350,10 +1722,10 @@
     <dataField name="Average of win by" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="5">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="0">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0" selected="0"/>
@@ -1694,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2104,10 +2476,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="K4:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2118,9 +2490,11 @@
     <col min="4" max="5" width="11.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2128,12 +2502,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" thickBot="1">
+    <row r="3" spans="1:14" ht="16" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" thickBot="1">
+    <row r="4" spans="1:14" ht="16" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2155,8 +2529,20 @@
       <c r="I4" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="K4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="4">
         <v>2008</v>
       </c>
@@ -2186,8 +2572,20 @@
         <f>H5-G5</f>
         <v>-11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="K5" s="23">
+        <v>2008</v>
+      </c>
+      <c r="L5" s="23">
+        <v>1647</v>
+      </c>
+      <c r="M5" s="23">
+        <v>1636</v>
+      </c>
+      <c r="N5" s="23">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="4">
         <v>2009</v>
       </c>
@@ -2217,8 +2615,20 @@
         <f t="shared" ref="I6:I10" si="4">H6-G6</f>
         <v>-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6" s="23">
+        <v>2009</v>
+      </c>
+      <c r="L6" s="23">
+        <v>1710</v>
+      </c>
+      <c r="M6" s="23">
+        <v>1708</v>
+      </c>
+      <c r="N6" s="23">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="4">
         <v>2010</v>
       </c>
@@ -2248,8 +2658,20 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="K7" s="24">
+        <v>2010</v>
+      </c>
+      <c r="L7" s="24">
+        <v>1590</v>
+      </c>
+      <c r="M7" s="24">
+        <v>1593</v>
+      </c>
+      <c r="N7" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="4">
         <v>2011</v>
       </c>
@@ -2279,8 +2701,20 @@
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="K8" s="24">
+        <v>2011</v>
+      </c>
+      <c r="L8" s="24">
+        <v>1670</v>
+      </c>
+      <c r="M8" s="24">
+        <v>1691</v>
+      </c>
+      <c r="N8" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="4">
         <v>2012</v>
       </c>
@@ -2310,8 +2744,20 @@
         <f t="shared" si="4"/>
         <v>-9</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="K9" s="23">
+        <v>2012</v>
+      </c>
+      <c r="L9" s="23">
+        <v>1632</v>
+      </c>
+      <c r="M9" s="23">
+        <v>1623</v>
+      </c>
+      <c r="N9" s="23">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="4">
         <v>2013</v>
       </c>
@@ -2341,8 +2787,20 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="K10" s="24">
+        <v>2013</v>
+      </c>
+      <c r="L10" s="24">
+        <v>1651</v>
+      </c>
+      <c r="M10" s="24">
+        <v>1655</v>
+      </c>
+      <c r="N10" s="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -2351,6 +2809,34 @@
       </c>
       <c r="C11" s="2">
         <v>6</v>
+      </c>
+      <c r="K11" s="24">
+        <v>2014</v>
+      </c>
+      <c r="L11" s="24">
+        <v>1657</v>
+      </c>
+      <c r="M11" s="24">
+        <v>1664</v>
+      </c>
+      <c r="N11" s="24">
+        <f>M11-L11</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="K12" s="23">
+        <v>2015</v>
+      </c>
+      <c r="L12" s="23">
+        <v>1507</v>
+      </c>
+      <c r="M12" s="23">
+        <v>1505</v>
+      </c>
+      <c r="N12" s="23">
+        <f>M12-L12</f>
+        <v>-2</v>
       </c>
     </row>
   </sheetData>
@@ -2366,10 +2852,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G29"/>
+  <dimension ref="A3:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="J5" sqref="J5:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2381,7 +2867,7 @@
     <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2389,7 +2875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2412,7 +2898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2434,8 +2920,24 @@
       <c r="G5" s="14">
         <v>54.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="J5" t="str">
+        <f>A5</f>
+        <v>2005-07</v>
+      </c>
+      <c r="K5">
+        <f>B5</f>
+        <v>2008</v>
+      </c>
+      <c r="L5" s="14">
+        <f>C5</f>
+        <v>-11</v>
+      </c>
+      <c r="M5" s="14">
+        <f>E5</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2457,8 +2959,24 @@
       <c r="G6" s="14">
         <v>23.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="J6" t="str">
+        <f t="shared" ref="J6:J10" si="0">A6</f>
+        <v>2006-08</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K10" si="1">B6</f>
+        <v>2009</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" ref="L6:L10" si="2">C6</f>
+        <v>-2</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" ref="M6:M10" si="3">E6</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2480,8 +2998,24 @@
       <c r="G7" s="14">
         <v>40.75</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>2007-09</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>2010</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2503,8 +3037,24 @@
       <c r="G8" s="14">
         <v>36.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>2008-10</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>2011</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2526,8 +3076,24 @@
       <c r="G9" s="14">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>2009-11</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>2012</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2549,8 +3115,24 @@
       <c r="G10" s="14">
         <v>26.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>2010-12</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>2013</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2569,22 +3151,30 @@
       <c r="G11" s="14">
         <v>30.625</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="L11" s="28">
+        <f>AVERAGE(L5:L10)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M11" s="14">
+        <f>AVERAGE(M5:M10)</f>
+        <v>43.333333333333336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="C12" s="3">
         <f>STDEV(C5:C10)</f>
         <v>11.465891446663303</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" ref="D12:F12" si="0">STDEV(D5:D10)</f>
+        <f t="shared" ref="D12:F12" si="4">STDEV(D5:D10)</f>
         <v>28.267767274170538</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>20.915703829100917</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>22.710496838833507</v>
       </c>
     </row>
@@ -2820,8 +3410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:G55"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4052,6 +4642,810 @@
     </row>
     <row r="56" spans="1:7" ht="17">
       <c r="C56" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="4" spans="1:4" ht="32">
+      <c r="A4" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16">
+      <c r="A5" s="26">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="26">
+        <v>2008</v>
+      </c>
+      <c r="C5" s="26">
+        <v>-11</v>
+      </c>
+      <c r="D5" s="26">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16">
+      <c r="A6" s="26">
+        <v>2013</v>
+      </c>
+      <c r="B6" s="26">
+        <v>2009</v>
+      </c>
+      <c r="C6" s="26">
+        <v>-2</v>
+      </c>
+      <c r="D6" s="26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="26">
+        <v>2013</v>
+      </c>
+      <c r="B7" s="26">
+        <v>2010</v>
+      </c>
+      <c r="C7" s="26">
+        <v>3</v>
+      </c>
+      <c r="D7" s="26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" s="26">
+        <v>2013</v>
+      </c>
+      <c r="B8" s="26">
+        <v>2011</v>
+      </c>
+      <c r="C8" s="26">
+        <v>21</v>
+      </c>
+      <c r="D8" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16">
+      <c r="A9" s="26">
+        <v>2013</v>
+      </c>
+      <c r="B9" s="26">
+        <v>2012</v>
+      </c>
+      <c r="C9" s="26">
+        <v>-9</v>
+      </c>
+      <c r="D9" s="26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16">
+      <c r="A10" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27">
+        <f>AVERAGE(C5:C9)</f>
+        <v>0.4</v>
+      </c>
+      <c r="D10" s="27">
+        <f>AVERAGE(D5:D9)</f>
+        <v>34.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:I32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" ht="18">
+      <c r="A3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17">
+      <c r="A4" s="11">
+        <v>9</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.815774</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17">
+      <c r="A5" s="11">
+        <v>9</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.80022300000000002</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17">
+      <c r="A6" s="11">
+        <v>9</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="11">
+        <v>6</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.72904100000000005</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17">
+      <c r="A7" s="11">
+        <v>9</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="11">
+        <v>7</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.72206099999999995</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17">
+      <c r="A8" s="11">
+        <v>9</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="11">
+        <v>7</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.68529399999999996</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17">
+      <c r="A9" s="11">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.61577700000000002</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.59486000000000006</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.56856700000000004</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17">
+      <c r="A12" s="11">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.56584999999999996</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17">
+      <c r="A13" s="11">
+        <v>9</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="11">
+        <v>5</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.56564899999999996</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17">
+      <c r="A14" s="11">
+        <v>9</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="11">
+        <v>3</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.52841300000000002</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17">
+      <c r="A15" s="11">
+        <v>9</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.51038099999999997</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17">
+      <c r="A16" s="11">
+        <v>9</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.44110500000000002</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="17" customFormat="1" ht="36">
+      <c r="A19" s="29"/>
+      <c r="B19" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="17">
+      <c r="A20" s="11"/>
+      <c r="B20" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="32">
+        <v>0.815774</v>
+      </c>
+      <c r="D20" s="31">
+        <v>16</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="31">
+        <v>16</v>
+      </c>
+      <c r="G20" s="31">
+        <v>7.5</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17">
+      <c r="A21" s="11"/>
+      <c r="B21" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="32">
+        <v>0.80022300000000002</v>
+      </c>
+      <c r="D21" s="31">
+        <v>15</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="31">
+        <v>15</v>
+      </c>
+      <c r="G21" s="31">
+        <v>-7.5</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17">
+      <c r="A22" s="11"/>
+      <c r="B22" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="32">
+        <v>0.72904100000000005</v>
+      </c>
+      <c r="D22" s="31">
+        <v>14</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="31">
+        <v>12</v>
+      </c>
+      <c r="G22" s="31">
+        <v>6</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="17">
+      <c r="A23" s="11"/>
+      <c r="B23" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="32">
+        <v>0.72206099999999995</v>
+      </c>
+      <c r="D23" s="31">
+        <v>13</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="31">
+        <v>13</v>
+      </c>
+      <c r="G23" s="31">
+        <v>7</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17">
+      <c r="A24" s="11"/>
+      <c r="B24" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="32">
+        <v>0.68529399999999996</v>
+      </c>
+      <c r="D24" s="31">
+        <v>12</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="31">
+        <v>14</v>
+      </c>
+      <c r="G24" s="31">
+        <v>7</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="17">
+      <c r="A25" s="11"/>
+      <c r="B25" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="32">
+        <v>0.61577700000000002</v>
+      </c>
+      <c r="D25" s="31">
+        <v>11</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="31">
+        <v>9</v>
+      </c>
+      <c r="G25" s="31">
+        <v>-3.5</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17">
+      <c r="A26" s="11"/>
+      <c r="B26" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="32">
+        <v>0.59486000000000006</v>
+      </c>
+      <c r="D26" s="31">
+        <v>10</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="31">
+        <v>8</v>
+      </c>
+      <c r="G26" s="31">
+        <v>-3.5</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="17">
+      <c r="A27" s="11"/>
+      <c r="B27" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="32">
+        <v>0.56856700000000004</v>
+      </c>
+      <c r="D27" s="31">
+        <v>9</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="31">
+        <v>6</v>
+      </c>
+      <c r="G27" s="31">
+        <v>2.5</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="17">
+      <c r="A28" s="11"/>
+      <c r="B28" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="32">
+        <v>0.56584999999999996</v>
+      </c>
+      <c r="D28" s="31">
+        <v>8</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="31">
+        <v>10</v>
+      </c>
+      <c r="G28" s="31">
+        <v>3.5</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17">
+      <c r="A29" s="11"/>
+      <c r="B29" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="32">
+        <v>0.56564899999999996</v>
+      </c>
+      <c r="D29" s="31">
+        <v>7</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="31">
+        <v>11</v>
+      </c>
+      <c r="G29" s="31">
+        <v>5</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="17">
+      <c r="A30" s="11"/>
+      <c r="B30" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="32">
+        <v>0.52841300000000002</v>
+      </c>
+      <c r="D30" s="31">
+        <v>6</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="31">
+        <v>7</v>
+      </c>
+      <c r="G30" s="31">
+        <v>-3</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17">
+      <c r="A31" s="11"/>
+      <c r="B31" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="32">
+        <v>0.51038099999999997</v>
+      </c>
+      <c r="D31" s="31">
+        <v>5</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="31">
+        <v>5</v>
+      </c>
+      <c r="G31" s="31">
+        <v>0</v>
+      </c>
+      <c r="H31" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="17">
+      <c r="A32" s="11"/>
+      <c r="B32" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="32">
+        <v>0.44110500000000002</v>
+      </c>
+      <c r="D32" s="31">
+        <v>4</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="31">
+        <v>4</v>
+      </c>
+      <c r="G32" s="31">
+        <v>0</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" s="33" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>